<commit_message>
Statistics for standard and naive Splay tree
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -155,7 +155,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>4</a:t>
+              <a:t>4: sequence test</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -562,11 +562,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1838610272"/>
-        <c:axId val="-1838603744"/>
+        <c:axId val="-1667455536"/>
+        <c:axId val="-1667467504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1838610272"/>
+        <c:axId val="-1667455536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838603744"/>
+        <c:crossAx val="-1667467504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -617,7 +617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1838603744"/>
+        <c:axId val="-1667467504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838610272"/>
+        <c:crossAx val="-1667455536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13134,11 +13134,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1838777840"/>
-        <c:axId val="-1690578960"/>
+        <c:axId val="-1667454992"/>
+        <c:axId val="-1667454448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1838777840"/>
+        <c:axId val="-1667454992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13181,7 +13181,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1690578960"/>
+        <c:crossAx val="-1667454448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13189,7 +13189,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1690578960"/>
+        <c:axId val="-1667454448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13240,7 +13240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838777840"/>
+        <c:crossAx val="-1667454992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25706,11 +25706,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1690578416"/>
-        <c:axId val="-1690577872"/>
+        <c:axId val="-1667464240"/>
+        <c:axId val="-1667457168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1690578416"/>
+        <c:axId val="-1667464240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25753,7 +25753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1690577872"/>
+        <c:crossAx val="-1667457168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25761,7 +25761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1690577872"/>
+        <c:axId val="-1667457168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25812,7 +25812,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1690578416"/>
+        <c:crossAx val="-1667464240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -38278,11 +38278,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1575965936"/>
-        <c:axId val="-1575956144"/>
+        <c:axId val="-1667453904"/>
+        <c:axId val="-1667453360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1575965936"/>
+        <c:axId val="-1667453904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -38325,7 +38325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1575956144"/>
+        <c:crossAx val="-1667453360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -38333,7 +38333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1575956144"/>
+        <c:axId val="-1667453360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -38384,7 +38384,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1575965936"/>
+        <c:crossAx val="-1667453904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -40773,15 +40773,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>348792</xdr:colOff>
+      <xdr:colOff>386499</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>169682</xdr:rowOff>
+      <xdr:rowOff>122548</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>94268</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>443060</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>84841</xdr:rowOff>
+      <xdr:rowOff>37707</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -41070,8 +41070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>

</xml_diff>